<commit_message>
feedstuffs added in excel, then done alright
</commit_message>
<xml_diff>
--- a/assets/Sir Mubarak data/UVA GRO Inclusion levels.xlsx
+++ b/assets/Sir Mubarak data/UVA GRO Inclusion levels.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2. Research\Projects\uvas ttsf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\donewithit\assets\Sir Mubarak data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3084FFA-A3AA-4920-AB32-C9121C29293F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Composition Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="clean composition" sheetId="2" r:id="rId2"/>
     <sheet name="Composition April 8, 2023" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="More Feedstuffs added" sheetId="7" r:id="rId4"/>
+    <sheet name="Final Feedstuffs" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="94">
   <si>
     <t>Barseem</t>
   </si>
@@ -249,12 +250,69 @@
   <si>
     <t>Cow pea (Rawanhan)</t>
   </si>
+  <si>
+    <t>Grains</t>
+  </si>
+  <si>
+    <t>Millet Grains</t>
+  </si>
+  <si>
+    <t>Rice Grains</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oats Grains</t>
+  </si>
+  <si>
+    <t>Barley Grains</t>
+  </si>
+  <si>
+    <t>Sorghum Grains</t>
+  </si>
+  <si>
+    <t>Cane Molasses</t>
+  </si>
+  <si>
+    <t>Fodders</t>
+  </si>
+  <si>
+    <t>Barseem Hay</t>
+  </si>
+  <si>
+    <t>Cowpea Hay</t>
+  </si>
+  <si>
+    <t>Millet Straw</t>
+  </si>
+  <si>
+    <t>Cowpea Mature</t>
+  </si>
+  <si>
+    <t>Napier Grass Mature</t>
+  </si>
+  <si>
+    <t>Fenugreek Early Vegetative</t>
+  </si>
+  <si>
+    <t>Sorghum Silage</t>
+  </si>
+  <si>
+    <t>Rhodes Grass</t>
+  </si>
+  <si>
+    <t>Sugarcane Bagasse</t>
+  </si>
+  <si>
+    <t>Lucerne Hay</t>
+  </si>
+  <si>
+    <t>Newly Added Feedstuffs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +326,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,8 +373,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -318,11 +440,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -357,6 +559,80 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1762,7 +2038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3226,11 +3502,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView topLeftCell="A51" zoomScale="76" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,13 +4978,4302 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="15"/>
+      <c r="C52" s="16">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D52" s="15">
+        <v>10.9</v>
+      </c>
+      <c r="E52" s="16">
+        <v>3</v>
+      </c>
+      <c r="F52" s="15">
+        <v>3000</v>
+      </c>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="15"/>
+      <c r="C53" s="16">
+        <v>12</v>
+      </c>
+      <c r="D53" s="15">
+        <v>20</v>
+      </c>
+      <c r="E53" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="F53" s="15">
+        <v>2800</v>
+      </c>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="15"/>
+      <c r="C54" s="16">
+        <v>11</v>
+      </c>
+      <c r="D54" s="15">
+        <v>13.8</v>
+      </c>
+      <c r="E54" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="F54" s="15">
+        <v>2600</v>
+      </c>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16">
+        <v>9</v>
+      </c>
+      <c r="D55" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="E55" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="F55" s="15">
+        <v>2800</v>
+      </c>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="16">
+        <v>12</v>
+      </c>
+      <c r="D56" s="15">
+        <v>15.3</v>
+      </c>
+      <c r="E56" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F56" s="15">
+        <v>2200</v>
+      </c>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="15"/>
+      <c r="C57" s="16">
+        <v>2</v>
+      </c>
+      <c r="D57" s="15">
+        <v>0</v>
+      </c>
+      <c r="E57" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="F57" s="15">
+        <v>2600</v>
+      </c>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="16">
+        <v>15</v>
+      </c>
+      <c r="D59" s="17">
+        <v>49.6</v>
+      </c>
+      <c r="E59" s="16">
+        <v>2.4</v>
+      </c>
+      <c r="F59" s="17">
+        <v>2400</v>
+      </c>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="16">
+        <v>16</v>
+      </c>
+      <c r="D60" s="17">
+        <v>43.6</v>
+      </c>
+      <c r="E60" s="16">
+        <v>2</v>
+      </c>
+      <c r="F60" s="17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="16">
+        <v>15</v>
+      </c>
+      <c r="D61" s="17">
+        <v>54</v>
+      </c>
+      <c r="E61" s="16">
+        <v>1.8</v>
+      </c>
+      <c r="F61" s="17">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="16">
+        <v>4</v>
+      </c>
+      <c r="D62" s="17">
+        <v>78</v>
+      </c>
+      <c r="E62" s="16">
+        <v>1.7</v>
+      </c>
+      <c r="F62" s="17">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="D63" s="17">
+        <v>46.3</v>
+      </c>
+      <c r="E63" s="16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F63" s="17">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="16">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D64" s="17">
+        <v>71.7</v>
+      </c>
+      <c r="E64" s="16">
+        <v>1.9</v>
+      </c>
+      <c r="F64" s="17">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="16">
+        <v>15.7</v>
+      </c>
+      <c r="D65" s="17">
+        <v>0</v>
+      </c>
+      <c r="E65" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="F65" s="17">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="D66" s="17">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="E66" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="F66" s="17">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="16">
+        <v>9.4</v>
+      </c>
+      <c r="D67" s="17">
+        <v>72</v>
+      </c>
+      <c r="E67" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="F67" s="17">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="E68" s="16">
+        <v>1.3</v>
+      </c>
+      <c r="F68" s="17">
+        <v>1300</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I68"/>
+  <sheetViews>
+    <sheetView zoomScale="78" workbookViewId="0">
+      <selection activeCell="E20" sqref="A1:I68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16">
+        <v>12.5</v>
+      </c>
+      <c r="C2" s="16">
+        <v>23.5</v>
+      </c>
+      <c r="D2" s="16">
+        <v>44.1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F2" s="23">
+        <f t="shared" ref="F2:F49" si="0">E2*1000</f>
+        <v>2300</v>
+      </c>
+      <c r="G2" s="24">
+        <v>12</v>
+      </c>
+      <c r="H2" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="16">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>39.9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F3" s="12">
+        <v>2246</v>
+      </c>
+      <c r="G3" s="5">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D4" s="4">
+        <v>71.5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1950</v>
+      </c>
+      <c r="G4" s="5">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="4">
+        <v>13.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43.5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="F5" s="12">
+        <v>2400</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4">
+        <v>12.4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.19</v>
+      </c>
+      <c r="F6" s="12">
+        <v>2190</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="4">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.19</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2190</v>
+      </c>
+      <c r="G7" s="5">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16">
+        <v>23.3</v>
+      </c>
+      <c r="C8" s="16">
+        <v>8.9</v>
+      </c>
+      <c r="D8" s="16">
+        <v>59.5</v>
+      </c>
+      <c r="E8" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8" s="23">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G8" s="24">
+        <v>5</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D9" s="4">
+        <v>57.9</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>2100</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4">
+        <v>26.3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>51.4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G10" s="5">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>29.6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D12" s="4">
+        <v>58.5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G12" s="5">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>51.1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G13" s="5">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="4">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5">
+        <v>24.4</v>
+      </c>
+      <c r="D14" s="4">
+        <v>27.1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.74</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="0"/>
+        <v>2740</v>
+      </c>
+      <c r="G14" s="5">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="C15" s="5">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.34</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>2340</v>
+      </c>
+      <c r="G15" s="5">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>26.8</v>
+      </c>
+      <c r="C16" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="G16" s="5">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C17" s="4">
+        <v>11.6</v>
+      </c>
+      <c r="D17" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5">
+        <v>91</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="D18" s="4">
+        <v>71.8</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G18" s="5">
+        <v>17</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4">
+        <v>92.8</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>66.5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="G19" s="5">
+        <v>8</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4">
+        <v>93.1</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4">
+        <v>72.2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G20" s="5">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4">
+        <v>92.9</v>
+      </c>
+      <c r="C21" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>70.2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G21" s="5">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4">
+        <v>85.5</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="D22" s="4">
+        <v>68.3</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="F22" s="12">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="G22" s="5">
+        <v>5</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4">
+        <v>91.5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="D23" s="4">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="F23" s="12">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+      <c r="G23" s="5">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="4">
+        <v>91.9</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="D24" s="4">
+        <v>63.7</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G24" s="5">
+        <v>15</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="4">
+        <v>87.3</v>
+      </c>
+      <c r="C25" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="D25" s="4">
+        <v>10.6</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="F25" s="12">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="G25" s="5">
+        <v>75</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="20">
+        <v>87</v>
+      </c>
+      <c r="C26" s="21">
+        <v>14.4</v>
+      </c>
+      <c r="D26" s="21">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E26" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="F26" s="22">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="G26" s="20">
+        <v>100</v>
+      </c>
+      <c r="H26" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="4">
+        <v>89.6</v>
+      </c>
+      <c r="C27" s="4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D27" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="F27" s="12">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="G27" s="5">
+        <v>100</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4">
+        <v>87.5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>12.8</v>
+      </c>
+      <c r="D28" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F28" s="12">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+      <c r="G28" s="5">
+        <v>50</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5">
+        <v>89</v>
+      </c>
+      <c r="C29" s="5">
+        <v>10</v>
+      </c>
+      <c r="D29" s="4">
+        <v>40.5</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="F29" s="12">
+        <f t="shared" si="0"/>
+        <v>2600</v>
+      </c>
+      <c r="G29" s="5">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="5">
+        <v>87</v>
+      </c>
+      <c r="C30" s="4">
+        <v>15.9</v>
+      </c>
+      <c r="D30" s="4">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F30" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G30" s="5">
+        <v>45</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="4">
+        <v>90.2</v>
+      </c>
+      <c r="C31" s="4">
+        <v>15.9</v>
+      </c>
+      <c r="D31" s="4">
+        <v>24.7</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F31" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G31" s="5">
+        <v>30</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="5">
+        <v>21</v>
+      </c>
+      <c r="C32" s="4">
+        <v>10.7</v>
+      </c>
+      <c r="D32" s="4">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="F32" s="12">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="G32" s="5">
+        <v>50</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="C33" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D33" s="4">
+        <v>53.5</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F33" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G33" s="5">
+        <v>20</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="5">
+        <v>23</v>
+      </c>
+      <c r="C34" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="D34" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G34" s="5">
+        <v>20</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="5">
+        <v>89</v>
+      </c>
+      <c r="C35" s="4">
+        <v>15.3</v>
+      </c>
+      <c r="D35" s="4">
+        <v>26.8</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="G35" s="5">
+        <v>65</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="4">
+        <v>88.6</v>
+      </c>
+      <c r="C36" s="4">
+        <v>16.8</v>
+      </c>
+      <c r="D36" s="4">
+        <v>31.6</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G36" s="5">
+        <v>65</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="4">
+        <v>87.9</v>
+      </c>
+      <c r="C37" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="D37" s="4">
+        <v>28.6</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G37" s="5">
+        <v>65</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="5">
+        <v>84</v>
+      </c>
+      <c r="C38" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="D38" s="4">
+        <v>27.4</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G38" s="5">
+        <v>20</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="C39" s="4">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="D39" s="4">
+        <v>13.3</v>
+      </c>
+      <c r="E39" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F39" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G39" s="5">
+        <v>20</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="4">
+        <v>92.2</v>
+      </c>
+      <c r="C40" s="4">
+        <v>23.8</v>
+      </c>
+      <c r="D40" s="4">
+        <v>43.2</v>
+      </c>
+      <c r="E40" s="5">
+        <v>2</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G40" s="5">
+        <v>100</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="4">
+        <v>87.9</v>
+      </c>
+      <c r="C41" s="5">
+        <v>48</v>
+      </c>
+      <c r="D41" s="4">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F41" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G41" s="5">
+        <v>300</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="4">
+        <v>88.8</v>
+      </c>
+      <c r="C42" s="4">
+        <v>39.6</v>
+      </c>
+      <c r="D42" s="4">
+        <v>31.2</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F42" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G42" s="5">
+        <v>145</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="4">
+        <v>90.6</v>
+      </c>
+      <c r="C43" s="4">
+        <v>34.1</v>
+      </c>
+      <c r="D43" s="4">
+        <v>25.4</v>
+      </c>
+      <c r="E43" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F43" s="12">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G43" s="5">
+        <v>145</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="4">
+        <v>89.9</v>
+      </c>
+      <c r="C44" s="4">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D44" s="4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E44" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F44" s="12">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="G44" s="5">
+        <v>130</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="4">
+        <v>88.3</v>
+      </c>
+      <c r="C45" s="5">
+        <v>29</v>
+      </c>
+      <c r="D45" s="4">
+        <v>30.6</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F45" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G45" s="5">
+        <v>61</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="5">
+        <v>90</v>
+      </c>
+      <c r="C46" s="4">
+        <v>59.7</v>
+      </c>
+      <c r="D46" s="5">
+        <v>18</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G46" s="5">
+        <v>40</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="4">
+        <v>91.2</v>
+      </c>
+      <c r="C47" s="4">
+        <v>17.8</v>
+      </c>
+      <c r="D47" s="5">
+        <v>57</v>
+      </c>
+      <c r="E47" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F47" s="12">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G47" s="5">
+        <v>50</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="5">
+        <v>89</v>
+      </c>
+      <c r="C48" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="D48" s="4">
+        <v>43.8</v>
+      </c>
+      <c r="E48" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F48" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G48" s="5">
+        <v>55</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="5">
+        <v>95</v>
+      </c>
+      <c r="C49" s="4">
+        <v>40.4</v>
+      </c>
+      <c r="D49" s="4">
+        <v>56.8</v>
+      </c>
+      <c r="E49" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F49" s="12">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="G49" s="5">
+        <v>120</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A50" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="26">
+        <v>87.4</v>
+      </c>
+      <c r="C52" s="16">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D52" s="15">
+        <v>10.9</v>
+      </c>
+      <c r="E52" s="16">
+        <v>3</v>
+      </c>
+      <c r="F52" s="15">
+        <v>3000</v>
+      </c>
+      <c r="G52" s="15">
+        <v>90</v>
+      </c>
+      <c r="H52" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="I52" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="26">
+        <v>87.1</v>
+      </c>
+      <c r="C53" s="16">
+        <v>12</v>
+      </c>
+      <c r="D53" s="15">
+        <v>20</v>
+      </c>
+      <c r="E53" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="F53" s="15">
+        <v>2800</v>
+      </c>
+      <c r="G53" s="15">
+        <v>90</v>
+      </c>
+      <c r="H53" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="I53" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="26">
+        <v>89.3</v>
+      </c>
+      <c r="C54" s="16">
+        <v>11</v>
+      </c>
+      <c r="D54" s="15">
+        <v>13.8</v>
+      </c>
+      <c r="E54" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="F54" s="15">
+        <v>2600</v>
+      </c>
+      <c r="G54" s="15">
+        <v>90</v>
+      </c>
+      <c r="H54" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="I54" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="26">
+        <v>87.5</v>
+      </c>
+      <c r="C55" s="16">
+        <v>9</v>
+      </c>
+      <c r="D55" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="E55" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="F55" s="15">
+        <v>2800</v>
+      </c>
+      <c r="G55" s="15">
+        <v>90</v>
+      </c>
+      <c r="H55" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="I55" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="26">
+        <v>89</v>
+      </c>
+      <c r="C56" s="16">
+        <v>12</v>
+      </c>
+      <c r="D56" s="15">
+        <v>15.3</v>
+      </c>
+      <c r="E56" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F56" s="15">
+        <v>2200</v>
+      </c>
+      <c r="G56" s="15">
+        <v>90</v>
+      </c>
+      <c r="H56" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="I56" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="26">
+        <v>73</v>
+      </c>
+      <c r="C57" s="16">
+        <v>2</v>
+      </c>
+      <c r="D57" s="15">
+        <v>0</v>
+      </c>
+      <c r="E57" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="F57" s="15">
+        <v>2600</v>
+      </c>
+      <c r="G57" s="15">
+        <v>90</v>
+      </c>
+      <c r="H57" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="I57" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="26">
+        <v>88.6</v>
+      </c>
+      <c r="C59" s="16">
+        <v>15</v>
+      </c>
+      <c r="D59" s="17">
+        <v>49.6</v>
+      </c>
+      <c r="E59" s="16">
+        <v>2.4</v>
+      </c>
+      <c r="F59" s="17">
+        <v>2400</v>
+      </c>
+      <c r="G59" s="24">
+        <v>12</v>
+      </c>
+      <c r="H59" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="I59" s="16">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="27">
+        <v>89.4</v>
+      </c>
+      <c r="C60" s="16">
+        <v>16</v>
+      </c>
+      <c r="D60" s="17">
+        <v>43.6</v>
+      </c>
+      <c r="E60" s="16">
+        <v>2</v>
+      </c>
+      <c r="F60" s="17">
+        <v>2000</v>
+      </c>
+      <c r="G60" s="5">
+        <v>5</v>
+      </c>
+      <c r="H60" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="26">
+        <v>91.2</v>
+      </c>
+      <c r="C61" s="16">
+        <v>15</v>
+      </c>
+      <c r="D61" s="17">
+        <v>54</v>
+      </c>
+      <c r="E61" s="16">
+        <v>1.8</v>
+      </c>
+      <c r="F61" s="17">
+        <v>1800</v>
+      </c>
+      <c r="G61" s="5">
+        <v>5</v>
+      </c>
+      <c r="H61" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I61" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="15">
+        <v>90</v>
+      </c>
+      <c r="C62" s="16">
+        <v>4</v>
+      </c>
+      <c r="D62" s="17">
+        <v>78</v>
+      </c>
+      <c r="E62" s="16">
+        <v>1.7</v>
+      </c>
+      <c r="F62" s="17">
+        <v>1700</v>
+      </c>
+      <c r="G62" s="5">
+        <v>5</v>
+      </c>
+      <c r="H62" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="26">
+        <v>20.9</v>
+      </c>
+      <c r="C63" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="D63" s="17">
+        <v>46.3</v>
+      </c>
+      <c r="E63" s="16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F63" s="17">
+        <v>2300</v>
+      </c>
+      <c r="G63" s="5">
+        <v>5</v>
+      </c>
+      <c r="H63" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I63" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="16">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D64" s="17">
+        <v>71.7</v>
+      </c>
+      <c r="E64" s="16">
+        <v>1.9</v>
+      </c>
+      <c r="F64" s="17">
+        <v>1900</v>
+      </c>
+      <c r="G64" s="5">
+        <v>5</v>
+      </c>
+      <c r="H64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="26">
+        <v>30.8</v>
+      </c>
+      <c r="C65" s="16">
+        <v>15.7</v>
+      </c>
+      <c r="D65" s="17">
+        <v>0</v>
+      </c>
+      <c r="E65" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="F65" s="17">
+        <v>2100</v>
+      </c>
+      <c r="G65" s="5">
+        <v>5</v>
+      </c>
+      <c r="H65" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I65" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" s="15">
+        <v>30</v>
+      </c>
+      <c r="C66" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="D66" s="17">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="E66" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="F66" s="17">
+        <v>2100</v>
+      </c>
+      <c r="G66" s="5">
+        <v>5</v>
+      </c>
+      <c r="H66" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I66" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67" s="26">
+        <v>24.9</v>
+      </c>
+      <c r="C67" s="16">
+        <v>9.4</v>
+      </c>
+      <c r="D67" s="17">
+        <v>72</v>
+      </c>
+      <c r="E67" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="F67" s="17">
+        <v>2100</v>
+      </c>
+      <c r="G67" s="5">
+        <v>5</v>
+      </c>
+      <c r="H67" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I67" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="26">
+        <v>46</v>
+      </c>
+      <c r="C68" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="D68" s="26">
+        <v>86.9</v>
+      </c>
+      <c r="E68" s="16">
+        <v>1.3</v>
+      </c>
+      <c r="F68" s="17">
+        <v>1300</v>
+      </c>
+      <c r="G68" s="5">
+        <v>5</v>
+      </c>
+      <c r="H68" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I68" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A50:I50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29">
+        <v>12.5</v>
+      </c>
+      <c r="C2" s="29">
+        <v>23.5</v>
+      </c>
+      <c r="D2" s="29">
+        <v>44.1</v>
+      </c>
+      <c r="E2" s="29">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F2" s="30">
+        <f t="shared" ref="F2:F49" si="0">E2*1000</f>
+        <v>2300</v>
+      </c>
+      <c r="G2" s="31">
+        <v>12</v>
+      </c>
+      <c r="H2" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>39.9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F3" s="12">
+        <v>2246</v>
+      </c>
+      <c r="G3" s="5">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D4" s="4">
+        <v>71.5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1950</v>
+      </c>
+      <c r="G4" s="5">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="4">
+        <v>13.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43.5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="F5" s="12">
+        <v>2400</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4">
+        <v>12.4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.19</v>
+      </c>
+      <c r="F6" s="12">
+        <v>2190</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="4">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.19</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2190</v>
+      </c>
+      <c r="G7" s="5">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="29">
+        <v>23.3</v>
+      </c>
+      <c r="C8" s="29">
+        <v>8.9</v>
+      </c>
+      <c r="D8" s="29">
+        <v>59.5</v>
+      </c>
+      <c r="E8" s="29">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8" s="30">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G8" s="31">
+        <v>5</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D9" s="4">
+        <v>57.9</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>2100</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4">
+        <v>26.3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>51.4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G10" s="5">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>29.6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D12" s="4">
+        <v>58.5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G12" s="5">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>51.1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G13" s="5">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="4">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5">
+        <v>24.4</v>
+      </c>
+      <c r="D14" s="4">
+        <v>27.1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.74</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="0"/>
+        <v>2740</v>
+      </c>
+      <c r="G14" s="5">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="C15" s="5">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.34</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>2340</v>
+      </c>
+      <c r="G15" s="5">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>26.8</v>
+      </c>
+      <c r="C16" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="G16" s="5">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C17" s="4">
+        <v>11.6</v>
+      </c>
+      <c r="D17" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5">
+        <v>91</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="D18" s="4">
+        <v>71.8</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G18" s="5">
+        <v>17</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4">
+        <v>92.8</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>66.5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="G19" s="5">
+        <v>8</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4">
+        <v>93.1</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4">
+        <v>72.2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G20" s="5">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4">
+        <v>92.9</v>
+      </c>
+      <c r="C21" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>70.2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G21" s="5">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4">
+        <v>85.5</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="D22" s="4">
+        <v>68.3</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="F22" s="12">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="G22" s="5">
+        <v>5</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4">
+        <v>91.5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="D23" s="4">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="F23" s="12">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+      <c r="G23" s="5">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="4">
+        <v>91.9</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="D24" s="4">
+        <v>63.7</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G24" s="5">
+        <v>15</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="4">
+        <v>87.3</v>
+      </c>
+      <c r="C25" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="D25" s="4">
+        <v>10.6</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="F25" s="12">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="G25" s="5">
+        <v>75</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="31">
+        <v>87</v>
+      </c>
+      <c r="C26" s="29">
+        <v>14.4</v>
+      </c>
+      <c r="D26" s="29">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E26" s="29">
+        <v>3.2</v>
+      </c>
+      <c r="F26" s="30">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="G26" s="31">
+        <v>100</v>
+      </c>
+      <c r="H26" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="I26" s="29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="4">
+        <v>89.6</v>
+      </c>
+      <c r="C27" s="4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D27" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="F27" s="12">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="G27" s="5">
+        <v>100</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4">
+        <v>87.5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>12.8</v>
+      </c>
+      <c r="D28" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F28" s="12">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+      <c r="G28" s="5">
+        <v>50</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5">
+        <v>89</v>
+      </c>
+      <c r="C29" s="5">
+        <v>10</v>
+      </c>
+      <c r="D29" s="4">
+        <v>40.5</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="F29" s="12">
+        <f t="shared" si="0"/>
+        <v>2600</v>
+      </c>
+      <c r="G29" s="5">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="5">
+        <v>87</v>
+      </c>
+      <c r="C30" s="4">
+        <v>15.9</v>
+      </c>
+      <c r="D30" s="4">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F30" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G30" s="5">
+        <v>45</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="4">
+        <v>90.2</v>
+      </c>
+      <c r="C31" s="4">
+        <v>15.9</v>
+      </c>
+      <c r="D31" s="4">
+        <v>24.7</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F31" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G31" s="5">
+        <v>30</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="5">
+        <v>21</v>
+      </c>
+      <c r="C32" s="4">
+        <v>10.7</v>
+      </c>
+      <c r="D32" s="4">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="F32" s="12">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="G32" s="5">
+        <v>50</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="C33" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D33" s="4">
+        <v>53.5</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F33" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G33" s="5">
+        <v>20</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="5">
+        <v>23</v>
+      </c>
+      <c r="C34" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="D34" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G34" s="5">
+        <v>20</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="5">
+        <v>89</v>
+      </c>
+      <c r="C35" s="4">
+        <v>15.3</v>
+      </c>
+      <c r="D35" s="4">
+        <v>26.8</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="G35" s="5">
+        <v>65</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="4">
+        <v>88.6</v>
+      </c>
+      <c r="C36" s="4">
+        <v>16.8</v>
+      </c>
+      <c r="D36" s="4">
+        <v>31.6</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="G36" s="5">
+        <v>65</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="4">
+        <v>87.9</v>
+      </c>
+      <c r="C37" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="D37" s="4">
+        <v>28.6</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G37" s="5">
+        <v>65</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="5">
+        <v>84</v>
+      </c>
+      <c r="C38" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="D38" s="4">
+        <v>27.4</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G38" s="5">
+        <v>20</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="C39" s="4">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="D39" s="4">
+        <v>13.3</v>
+      </c>
+      <c r="E39" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F39" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G39" s="5">
+        <v>20</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="4">
+        <v>92.2</v>
+      </c>
+      <c r="C40" s="4">
+        <v>23.8</v>
+      </c>
+      <c r="D40" s="4">
+        <v>43.2</v>
+      </c>
+      <c r="E40" s="5">
+        <v>2</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G40" s="5">
+        <v>100</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="4">
+        <v>87.9</v>
+      </c>
+      <c r="C41" s="5">
+        <v>48</v>
+      </c>
+      <c r="D41" s="4">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F41" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G41" s="5">
+        <v>300</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="4">
+        <v>88.8</v>
+      </c>
+      <c r="C42" s="4">
+        <v>39.6</v>
+      </c>
+      <c r="D42" s="4">
+        <v>31.2</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F42" s="12">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G42" s="5">
+        <v>145</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="4">
+        <v>90.6</v>
+      </c>
+      <c r="C43" s="4">
+        <v>34.1</v>
+      </c>
+      <c r="D43" s="4">
+        <v>25.4</v>
+      </c>
+      <c r="E43" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F43" s="12">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G43" s="5">
+        <v>145</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="4">
+        <v>89.9</v>
+      </c>
+      <c r="C44" s="4">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D44" s="4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E44" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F44" s="12">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="G44" s="5">
+        <v>130</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="4">
+        <v>88.3</v>
+      </c>
+      <c r="C45" s="5">
+        <v>29</v>
+      </c>
+      <c r="D45" s="4">
+        <v>30.6</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F45" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G45" s="5">
+        <v>61</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="5">
+        <v>90</v>
+      </c>
+      <c r="C46" s="4">
+        <v>59.7</v>
+      </c>
+      <c r="D46" s="5">
+        <v>18</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="G46" s="5">
+        <v>40</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="4">
+        <v>91.2</v>
+      </c>
+      <c r="C47" s="4">
+        <v>17.8</v>
+      </c>
+      <c r="D47" s="5">
+        <v>57</v>
+      </c>
+      <c r="E47" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F47" s="12">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="G47" s="5">
+        <v>50</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="5">
+        <v>89</v>
+      </c>
+      <c r="C48" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="D48" s="4">
+        <v>43.8</v>
+      </c>
+      <c r="E48" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="F48" s="12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G48" s="5">
+        <v>55</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="5">
+        <v>95</v>
+      </c>
+      <c r="C49" s="4">
+        <v>40.4</v>
+      </c>
+      <c r="D49" s="4">
+        <v>56.8</v>
+      </c>
+      <c r="E49" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F49" s="12">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="G49" s="5">
+        <v>120</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="33">
+        <v>87.4</v>
+      </c>
+      <c r="C50" s="34">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D50" s="35">
+        <v>10.9</v>
+      </c>
+      <c r="E50" s="34">
+        <v>3</v>
+      </c>
+      <c r="F50" s="35">
+        <v>3000</v>
+      </c>
+      <c r="G50" s="35">
+        <v>90</v>
+      </c>
+      <c r="H50" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="I50" s="36">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="38">
+        <v>87.1</v>
+      </c>
+      <c r="C51" s="39">
+        <v>12</v>
+      </c>
+      <c r="D51" s="40">
+        <v>20</v>
+      </c>
+      <c r="E51" s="39">
+        <v>2.8</v>
+      </c>
+      <c r="F51" s="40">
+        <v>2800</v>
+      </c>
+      <c r="G51" s="40">
+        <v>90</v>
+      </c>
+      <c r="H51" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="I51" s="41">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="38">
+        <v>89.3</v>
+      </c>
+      <c r="C52" s="39">
+        <v>11</v>
+      </c>
+      <c r="D52" s="40">
+        <v>13.8</v>
+      </c>
+      <c r="E52" s="39">
+        <v>2.6</v>
+      </c>
+      <c r="F52" s="40">
+        <v>2600</v>
+      </c>
+      <c r="G52" s="40">
+        <v>90</v>
+      </c>
+      <c r="H52" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="I52" s="41">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="38">
+        <v>87.5</v>
+      </c>
+      <c r="C53" s="39">
+        <v>9</v>
+      </c>
+      <c r="D53" s="40">
+        <v>12.5</v>
+      </c>
+      <c r="E53" s="39">
+        <v>2.8</v>
+      </c>
+      <c r="F53" s="40">
+        <v>2800</v>
+      </c>
+      <c r="G53" s="40">
+        <v>90</v>
+      </c>
+      <c r="H53" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="I53" s="41">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="38">
+        <v>89</v>
+      </c>
+      <c r="C54" s="39">
+        <v>12</v>
+      </c>
+      <c r="D54" s="40">
+        <v>15.3</v>
+      </c>
+      <c r="E54" s="39">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F54" s="40">
+        <v>2200</v>
+      </c>
+      <c r="G54" s="40">
+        <v>90</v>
+      </c>
+      <c r="H54" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="I54" s="41">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="38">
+        <v>73</v>
+      </c>
+      <c r="C55" s="39">
+        <v>2</v>
+      </c>
+      <c r="D55" s="40">
+        <v>0</v>
+      </c>
+      <c r="E55" s="39">
+        <v>2.6</v>
+      </c>
+      <c r="F55" s="40">
+        <v>2600</v>
+      </c>
+      <c r="G55" s="40">
+        <v>90</v>
+      </c>
+      <c r="H55" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="I55" s="41">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="38">
+        <v>88.6</v>
+      </c>
+      <c r="C56" s="39">
+        <v>15</v>
+      </c>
+      <c r="D56" s="40">
+        <v>49.6</v>
+      </c>
+      <c r="E56" s="39">
+        <v>2.4</v>
+      </c>
+      <c r="F56" s="40">
+        <v>2400</v>
+      </c>
+      <c r="G56" s="42">
+        <v>12</v>
+      </c>
+      <c r="H56" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I56" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="43">
+        <v>89.4</v>
+      </c>
+      <c r="C57" s="39">
+        <v>16</v>
+      </c>
+      <c r="D57" s="40">
+        <v>43.6</v>
+      </c>
+      <c r="E57" s="39">
+        <v>2</v>
+      </c>
+      <c r="F57" s="40">
+        <v>2000</v>
+      </c>
+      <c r="G57" s="42">
+        <v>5</v>
+      </c>
+      <c r="H57" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I57" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" s="38">
+        <v>91.2</v>
+      </c>
+      <c r="C58" s="39">
+        <v>15</v>
+      </c>
+      <c r="D58" s="40">
+        <v>54</v>
+      </c>
+      <c r="E58" s="39">
+        <v>1.8</v>
+      </c>
+      <c r="F58" s="40">
+        <v>1800</v>
+      </c>
+      <c r="G58" s="42">
+        <v>5</v>
+      </c>
+      <c r="H58" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I58" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="40">
+        <v>90</v>
+      </c>
+      <c r="C59" s="39">
+        <v>4</v>
+      </c>
+      <c r="D59" s="40">
+        <v>78</v>
+      </c>
+      <c r="E59" s="39">
+        <v>1.7</v>
+      </c>
+      <c r="F59" s="40">
+        <v>1700</v>
+      </c>
+      <c r="G59" s="42">
+        <v>5</v>
+      </c>
+      <c r="H59" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I59" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" s="38">
+        <v>20.9</v>
+      </c>
+      <c r="C60" s="39">
+        <v>25.5</v>
+      </c>
+      <c r="D60" s="40">
+        <v>46.3</v>
+      </c>
+      <c r="E60" s="39">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F60" s="40">
+        <v>2300</v>
+      </c>
+      <c r="G60" s="42">
+        <v>5</v>
+      </c>
+      <c r="H60" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I60" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="38">
+        <v>30.8</v>
+      </c>
+      <c r="C61" s="39">
+        <v>15.7</v>
+      </c>
+      <c r="D61" s="40">
+        <v>0</v>
+      </c>
+      <c r="E61" s="39">
+        <v>2.1</v>
+      </c>
+      <c r="F61" s="40">
+        <v>2100</v>
+      </c>
+      <c r="G61" s="42">
+        <v>5</v>
+      </c>
+      <c r="H61" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I61" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="40">
+        <v>30</v>
+      </c>
+      <c r="C62" s="39">
+        <v>5.9</v>
+      </c>
+      <c r="D62" s="40">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="E62" s="39">
+        <v>2.1</v>
+      </c>
+      <c r="F62" s="40">
+        <v>2100</v>
+      </c>
+      <c r="G62" s="42">
+        <v>5</v>
+      </c>
+      <c r="H62" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I62" s="41">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" s="38">
+        <v>24.9</v>
+      </c>
+      <c r="C63" s="39">
+        <v>9.4</v>
+      </c>
+      <c r="D63" s="40">
+        <v>72</v>
+      </c>
+      <c r="E63" s="39">
+        <v>2.1</v>
+      </c>
+      <c r="F63" s="40">
+        <v>2100</v>
+      </c>
+      <c r="G63" s="42">
+        <v>5</v>
+      </c>
+      <c r="H63" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="I63" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" s="45">
+        <v>46</v>
+      </c>
+      <c r="C64" s="46">
+        <v>3.5</v>
+      </c>
+      <c r="D64" s="45">
+        <v>86.9</v>
+      </c>
+      <c r="E64" s="46">
+        <v>1.3</v>
+      </c>
+      <c r="F64" s="47">
+        <v>1300</v>
+      </c>
+      <c r="G64" s="48">
+        <v>5</v>
+      </c>
+      <c r="H64" s="46">
+        <v>0.01</v>
+      </c>
+      <c r="I64" s="49">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>

</xml_diff>

<commit_message>
added more feedstuffs with translation
</commit_message>
<xml_diff>
--- a/assets/Sir Mubarak data/UVA GRO Inclusion levels.xlsx
+++ b/assets/Sir Mubarak data/UVA GRO Inclusion levels.xlsx
@@ -565,12 +565,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -632,6 +626,12 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5396,11 +5396,11 @@
       <c r="E2" s="16">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="21">
         <f t="shared" ref="F2:F49" si="0">E2*1000</f>
         <v>2300</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="22">
         <v>12</v>
       </c>
       <c r="H2" s="16">
@@ -5571,11 +5571,11 @@
       <c r="E8" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="21">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="22">
         <v>5</v>
       </c>
       <c r="H8" s="16">
@@ -6098,29 +6098,29 @@
       <c r="A26" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="18">
         <v>87</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="19">
         <v>14.4</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="19">
         <v>16.899999999999999</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="19">
         <v>3.2</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="20">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="18">
         <v>100</v>
       </c>
-      <c r="H26" s="21">
-        <v>0.05</v>
-      </c>
-      <c r="I26" s="21">
+      <c r="H26" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="I26" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -6815,17 +6815,17 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
@@ -6860,7 +6860,7 @@
       <c r="A52" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="26">
+      <c r="B52" s="24">
         <v>87.4</v>
       </c>
       <c r="C52" s="16">
@@ -6889,7 +6889,7 @@
       <c r="A53" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="26">
+      <c r="B53" s="24">
         <v>87.1</v>
       </c>
       <c r="C53" s="16">
@@ -6918,7 +6918,7 @@
       <c r="A54" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="26">
+      <c r="B54" s="24">
         <v>89.3</v>
       </c>
       <c r="C54" s="16">
@@ -6947,7 +6947,7 @@
       <c r="A55" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="26">
+      <c r="B55" s="24">
         <v>87.5</v>
       </c>
       <c r="C55" s="16">
@@ -6976,7 +6976,7 @@
       <c r="A56" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="26">
+      <c r="B56" s="24">
         <v>89</v>
       </c>
       <c r="C56" s="16">
@@ -7005,7 +7005,7 @@
       <c r="A57" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="26">
+      <c r="B57" s="24">
         <v>73</v>
       </c>
       <c r="C57" s="16">
@@ -7063,7 +7063,7 @@
       <c r="A59" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="26">
+      <c r="B59" s="24">
         <v>88.6</v>
       </c>
       <c r="C59" s="16">
@@ -7078,7 +7078,7 @@
       <c r="F59" s="17">
         <v>2400</v>
       </c>
-      <c r="G59" s="24">
+      <c r="G59" s="22">
         <v>12</v>
       </c>
       <c r="H59" s="16">
@@ -7092,7 +7092,7 @@
       <c r="A60" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="27">
+      <c r="B60" s="25">
         <v>89.4</v>
       </c>
       <c r="C60" s="16">
@@ -7121,7 +7121,7 @@
       <c r="A61" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="26">
+      <c r="B61" s="24">
         <v>91.2</v>
       </c>
       <c r="C61" s="16">
@@ -7179,7 +7179,7 @@
       <c r="A63" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="26">
+      <c r="B63" s="24">
         <v>20.9</v>
       </c>
       <c r="C63" s="16">
@@ -7205,7 +7205,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="23" t="s">
         <v>87</v>
       </c>
       <c r="B64" s="15"/>
@@ -7235,7 +7235,7 @@
       <c r="A65" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="26">
+      <c r="B65" s="24">
         <v>30.8</v>
       </c>
       <c r="C65" s="16">
@@ -7293,7 +7293,7 @@
       <c r="A67" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B67" s="26">
+      <c r="B67" s="24">
         <v>24.9</v>
       </c>
       <c r="C67" s="16">
@@ -7322,13 +7322,13 @@
       <c r="A68" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="26">
+      <c r="B68" s="24">
         <v>46</v>
       </c>
       <c r="C68" s="16">
         <v>3.5</v>
       </c>
-      <c r="D68" s="26">
+      <c r="D68" s="24">
         <v>86.9</v>
       </c>
       <c r="E68" s="16">
@@ -7361,7 +7361,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7399,32 +7399,32 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="27">
         <v>12.5</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="27">
         <v>23.5</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="27">
         <v>44.1</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="27">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="28">
         <f t="shared" ref="F2:F49" si="0">E2*1000</f>
         <v>2300</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="29">
         <v>12</v>
       </c>
-      <c r="H2" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="29">
+      <c r="H2" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="27">
         <v>0.2</v>
       </c>
     </row>
@@ -7574,32 +7574,32 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="27">
         <v>23.3</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="27">
         <v>8.9</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="27">
         <v>59.5</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="28">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="G8" s="31">
-        <v>5</v>
-      </c>
-      <c r="H8" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="I8" s="29">
+      <c r="G8" s="29">
+        <v>5</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="27">
         <v>0.4</v>
       </c>
     </row>
@@ -8113,32 +8113,32 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="29">
         <v>87</v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26" s="27">
         <v>14.4</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="27">
         <v>16.899999999999999</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="27">
         <v>3.2</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="28">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="29">
         <v>100</v>
       </c>
-      <c r="H26" s="29">
-        <v>0.05</v>
-      </c>
-      <c r="I26" s="29">
+      <c r="H26" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="I26" s="27">
         <v>0.2</v>
       </c>
     </row>
@@ -8833,437 +8833,437 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="33">
+      <c r="B50" s="31">
         <v>87.4</v>
       </c>
-      <c r="C50" s="34">
+      <c r="C50" s="32">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D50" s="35">
+      <c r="D50" s="33">
         <v>10.9</v>
       </c>
-      <c r="E50" s="34">
+      <c r="E50" s="32">
         <v>3</v>
       </c>
-      <c r="F50" s="35">
+      <c r="F50" s="33">
         <v>3000</v>
       </c>
-      <c r="G50" s="35">
+      <c r="G50" s="33">
         <v>90</v>
       </c>
-      <c r="H50" s="34">
-        <v>0.05</v>
-      </c>
-      <c r="I50" s="36">
+      <c r="H50" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="I50" s="34">
         <v>0.15</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="38">
+      <c r="B51" s="36">
         <v>87.1</v>
       </c>
-      <c r="C51" s="39">
+      <c r="C51" s="37">
         <v>12</v>
       </c>
-      <c r="D51" s="40">
+      <c r="D51" s="38">
         <v>20</v>
       </c>
-      <c r="E51" s="39">
+      <c r="E51" s="37">
         <v>2.8</v>
       </c>
-      <c r="F51" s="40">
+      <c r="F51" s="38">
         <v>2800</v>
       </c>
-      <c r="G51" s="40">
+      <c r="G51" s="38">
         <v>90</v>
       </c>
-      <c r="H51" s="39">
-        <v>0.05</v>
-      </c>
-      <c r="I51" s="41">
+      <c r="H51" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="I51" s="39">
         <v>0.15</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="38">
+      <c r="B52" s="36">
         <v>89.3</v>
       </c>
-      <c r="C52" s="39">
+      <c r="C52" s="37">
         <v>11</v>
       </c>
-      <c r="D52" s="40">
+      <c r="D52" s="38">
         <v>13.8</v>
       </c>
-      <c r="E52" s="39">
+      <c r="E52" s="37">
         <v>2.6</v>
       </c>
-      <c r="F52" s="40">
+      <c r="F52" s="38">
         <v>2600</v>
       </c>
-      <c r="G52" s="40">
+      <c r="G52" s="38">
         <v>90</v>
       </c>
-      <c r="H52" s="39">
-        <v>0.05</v>
-      </c>
-      <c r="I52" s="41">
+      <c r="H52" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="I52" s="39">
         <v>0.15</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="B53" s="38">
+      <c r="B53" s="36">
         <v>87.5</v>
       </c>
-      <c r="C53" s="39">
+      <c r="C53" s="37">
         <v>9</v>
       </c>
-      <c r="D53" s="40">
+      <c r="D53" s="38">
         <v>12.5</v>
       </c>
-      <c r="E53" s="39">
+      <c r="E53" s="37">
         <v>2.8</v>
       </c>
-      <c r="F53" s="40">
+      <c r="F53" s="38">
         <v>2800</v>
       </c>
-      <c r="G53" s="40">
+      <c r="G53" s="38">
         <v>90</v>
       </c>
-      <c r="H53" s="39">
-        <v>0.05</v>
-      </c>
-      <c r="I53" s="41">
+      <c r="H53" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="I53" s="39">
         <v>0.15</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="38">
+      <c r="B54" s="36">
         <v>89</v>
       </c>
-      <c r="C54" s="39">
+      <c r="C54" s="37">
         <v>12</v>
       </c>
-      <c r="D54" s="40">
+      <c r="D54" s="38">
         <v>15.3</v>
       </c>
-      <c r="E54" s="39">
+      <c r="E54" s="37">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F54" s="40">
+      <c r="F54" s="38">
         <v>2200</v>
       </c>
-      <c r="G54" s="40">
+      <c r="G54" s="38">
         <v>90</v>
       </c>
-      <c r="H54" s="39">
-        <v>0.05</v>
-      </c>
-      <c r="I54" s="41">
+      <c r="H54" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="I54" s="39">
         <v>0.15</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="38">
+      <c r="B55" s="36">
         <v>73</v>
       </c>
-      <c r="C55" s="39">
+      <c r="C55" s="37">
         <v>2</v>
       </c>
-      <c r="D55" s="40">
+      <c r="D55" s="38">
         <v>0</v>
       </c>
-      <c r="E55" s="39">
+      <c r="E55" s="37">
         <v>2.6</v>
       </c>
-      <c r="F55" s="40">
+      <c r="F55" s="38">
         <v>2600</v>
       </c>
-      <c r="G55" s="40">
+      <c r="G55" s="38">
         <v>90</v>
       </c>
-      <c r="H55" s="39">
-        <v>0.05</v>
-      </c>
-      <c r="I55" s="41">
+      <c r="H55" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="I55" s="39">
         <v>0.15</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="38">
+      <c r="B56" s="36">
         <v>88.6</v>
       </c>
-      <c r="C56" s="39">
+      <c r="C56" s="37">
         <v>15</v>
       </c>
-      <c r="D56" s="40">
+      <c r="D56" s="38">
         <v>49.6</v>
       </c>
-      <c r="E56" s="39">
+      <c r="E56" s="37">
         <v>2.4</v>
       </c>
-      <c r="F56" s="40">
+      <c r="F56" s="38">
         <v>2400</v>
       </c>
-      <c r="G56" s="42">
+      <c r="G56" s="40">
         <v>12</v>
       </c>
-      <c r="H56" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I56" s="41">
+      <c r="H56" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I56" s="39">
         <v>0.2</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="43">
+      <c r="B57" s="41">
         <v>89.4</v>
       </c>
-      <c r="C57" s="39">
+      <c r="C57" s="37">
         <v>16</v>
       </c>
-      <c r="D57" s="40">
+      <c r="D57" s="38">
         <v>43.6</v>
       </c>
-      <c r="E57" s="39">
+      <c r="E57" s="37">
         <v>2</v>
       </c>
-      <c r="F57" s="40">
+      <c r="F57" s="38">
         <v>2000</v>
       </c>
-      <c r="G57" s="42">
-        <v>5</v>
-      </c>
-      <c r="H57" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I57" s="41">
+      <c r="G57" s="40">
+        <v>5</v>
+      </c>
+      <c r="H57" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I57" s="39">
         <v>0.2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="38">
+      <c r="B58" s="36">
         <v>91.2</v>
       </c>
-      <c r="C58" s="39">
+      <c r="C58" s="37">
         <v>15</v>
       </c>
-      <c r="D58" s="40">
+      <c r="D58" s="38">
         <v>54</v>
       </c>
-      <c r="E58" s="39">
+      <c r="E58" s="37">
         <v>1.8</v>
       </c>
-      <c r="F58" s="40">
+      <c r="F58" s="38">
         <v>1800</v>
       </c>
-      <c r="G58" s="42">
-        <v>5</v>
-      </c>
-      <c r="H58" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I58" s="41">
+      <c r="G58" s="40">
+        <v>5</v>
+      </c>
+      <c r="H58" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I58" s="39">
         <v>0.2</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="40">
+      <c r="B59" s="38">
         <v>90</v>
       </c>
-      <c r="C59" s="39">
+      <c r="C59" s="37">
         <v>4</v>
       </c>
-      <c r="D59" s="40">
+      <c r="D59" s="38">
         <v>78</v>
       </c>
-      <c r="E59" s="39">
+      <c r="E59" s="37">
         <v>1.7</v>
       </c>
-      <c r="F59" s="40">
+      <c r="F59" s="38">
         <v>1700</v>
       </c>
-      <c r="G59" s="42">
-        <v>5</v>
-      </c>
-      <c r="H59" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I59" s="41">
+      <c r="G59" s="40">
+        <v>5</v>
+      </c>
+      <c r="H59" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I59" s="39">
         <v>0.2</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="38">
+      <c r="B60" s="36">
         <v>20.9</v>
       </c>
-      <c r="C60" s="39">
+      <c r="C60" s="37">
         <v>25.5</v>
       </c>
-      <c r="D60" s="40">
+      <c r="D60" s="38">
         <v>46.3</v>
       </c>
-      <c r="E60" s="39">
+      <c r="E60" s="37">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F60" s="40">
+      <c r="F60" s="38">
         <v>2300</v>
       </c>
-      <c r="G60" s="42">
-        <v>5</v>
-      </c>
-      <c r="H60" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I60" s="41">
+      <c r="G60" s="40">
+        <v>5</v>
+      </c>
+      <c r="H60" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I60" s="39">
         <v>0.2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="s">
+      <c r="A61" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="B61" s="38">
+      <c r="B61" s="36">
         <v>30.8</v>
       </c>
-      <c r="C61" s="39">
+      <c r="C61" s="37">
         <v>15.7</v>
       </c>
-      <c r="D61" s="40">
+      <c r="D61" s="38">
         <v>0</v>
       </c>
-      <c r="E61" s="39">
+      <c r="E61" s="37">
         <v>2.1</v>
       </c>
-      <c r="F61" s="40">
+      <c r="F61" s="38">
         <v>2100</v>
       </c>
-      <c r="G61" s="42">
-        <v>5</v>
-      </c>
-      <c r="H61" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I61" s="41">
+      <c r="G61" s="40">
+        <v>5</v>
+      </c>
+      <c r="H61" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I61" s="39">
         <v>0.2</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B62" s="40">
+      <c r="B62" s="38">
         <v>30</v>
       </c>
-      <c r="C62" s="39">
+      <c r="C62" s="37">
         <v>5.9</v>
       </c>
-      <c r="D62" s="40">
+      <c r="D62" s="38">
         <v>65.900000000000006</v>
       </c>
-      <c r="E62" s="39">
+      <c r="E62" s="37">
         <v>2.1</v>
       </c>
-      <c r="F62" s="40">
+      <c r="F62" s="38">
         <v>2100</v>
       </c>
-      <c r="G62" s="42">
-        <v>5</v>
-      </c>
-      <c r="H62" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I62" s="41">
+      <c r="G62" s="40">
+        <v>5</v>
+      </c>
+      <c r="H62" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I62" s="39">
         <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B63" s="38">
+      <c r="B63" s="36">
         <v>24.9</v>
       </c>
-      <c r="C63" s="39">
+      <c r="C63" s="37">
         <v>9.4</v>
       </c>
-      <c r="D63" s="40">
+      <c r="D63" s="38">
         <v>72</v>
       </c>
-      <c r="E63" s="39">
+      <c r="E63" s="37">
         <v>2.1</v>
       </c>
-      <c r="F63" s="40">
+      <c r="F63" s="38">
         <v>2100</v>
       </c>
-      <c r="G63" s="42">
-        <v>5</v>
-      </c>
-      <c r="H63" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="I63" s="41">
+      <c r="G63" s="40">
+        <v>5</v>
+      </c>
+      <c r="H63" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="I63" s="39">
         <v>0.2</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="44" t="s">
+      <c r="A64" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="45">
+      <c r="B64" s="43">
         <v>46</v>
       </c>
-      <c r="C64" s="46">
+      <c r="C64" s="44">
         <v>3.5</v>
       </c>
-      <c r="D64" s="45">
+      <c r="D64" s="43">
         <v>86.9</v>
       </c>
-      <c r="E64" s="46">
+      <c r="E64" s="44">
         <v>1.3</v>
       </c>
-      <c r="F64" s="47">
+      <c r="F64" s="45">
         <v>1300</v>
       </c>
-      <c r="G64" s="48">
-        <v>5</v>
-      </c>
-      <c r="H64" s="46">
+      <c r="G64" s="46">
+        <v>5</v>
+      </c>
+      <c r="H64" s="44">
         <v>0.01</v>
       </c>
-      <c r="I64" s="49">
+      <c r="I64" s="47">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>